<commit_message>
data access layer is seperated..
</commit_message>
<xml_diff>
--- a/src/PivotTableInMVC/Content/ProductReport.xlsx
+++ b/src/PivotTableInMVC/Content/ProductReport.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raviteja\My Visual Studio Projects\mitechdev applications\PivotTableInMVC\PivotTableInMVC\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\PivotTableInExcel\src\PivotTableInMVC\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9885"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot Table" sheetId="2" r:id="rId1"/>
@@ -236,7 +236,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Admin" refreshedDate="42993.774709953701" createdVersion="1" refreshedVersion="5" recordCount="14">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="RavitejaSwayampu" refreshedDate="42996.352691203705" createdVersion="1" refreshedVersion="5" recordCount="14">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E15" sheet="ProductReport"/>
   </cacheSource>

</xml_diff>